<commit_message>
Atualização dos arquivos Excel e nova versão do main.py
</commit_message>
<xml_diff>
--- a/data/DIA_DE_SORTE.xlsx
+++ b/data/DIA_DE_SORTE.xlsx
@@ -87686,6 +87686,83 @@
         <x:v/>
       </x:c>
     </x:row>
+    <x:row>
+      <x:c t="n">
+        <x:v>1132</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>23/10/2025</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>04</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>06</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Janeiro</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>IGARASSU/PE</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$4.761.847,69</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$2.063,28</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>5707</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$25,00</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>60760</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$5,00</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>159250</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$2,50</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Não</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$5.164.162,50</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>R$200.000,00</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="2" type="noConversion"/>
   <x:pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -87874,7 +87951,7 @@
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-10-23T04:12:28+00:00</AtualizadoPeloTimerJobEm>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-10-24T04:12:12+00:00</AtualizadoPeloTimerJobEm>
   </documentManagement>
 </p:properties>
 </file>

</xml_diff>